<commit_message>
Enhance student timetable generation by adding logic to skip MasterClass activities that do not include the current student, improving the relevance of scheduled activities. Update multiple teacher timetable files to reflect recent changes.
</commit_message>
<xml_diff>
--- a/teacher_timetables/Gwyneth WENTINK_CampA_timetable.xlsx
+++ b/teacher_timetables/Gwyneth WENTINK_CampA_timetable.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Full Timetable" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Full Timetable" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>